<commit_message>
docs(progress/week_10): add more feature docs
* Teacher: approval

Closes: #15
Signed-off-by: Rong "Mantle" Bao <webmaster@csmantle.top>
</commit_message>
<xml_diff>
--- a/docs/progress/week_10/功能分析表.xlsx
+++ b/docs/progress/week_10/功能分析表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\hdu2025_software_eng_thesis_mgmt\docs\progress\week_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C246848B-911F-43A4-A426-CD7003682DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD535F46-1422-4F0B-B22A-591CA18ADFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,13 @@
     <sheet name="功能项清单" sheetId="9" r:id="rId1"/>
     <sheet name="1. 学生选题" sheetId="22" r:id="rId2"/>
     <sheet name="3. 教师课题申报" sheetId="23" r:id="rId3"/>
-    <sheet name="6. 答辩组答辩过程管理" sheetId="24" r:id="rId4"/>
+    <sheet name="4. 教师选题管理" sheetId="25" r:id="rId4"/>
+    <sheet name="6. 答辩组答辩过程管理" sheetId="24" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="表_学生选题">'1. 学生选题'!$A$1</definedName>
     <definedName name="表_教师课题申报">'3. 教师课题申报'!$A$1</definedName>
+    <definedName name="表_教师选题管理">'4. 教师选题管理'!$C$1</definedName>
     <definedName name="表_答辩组答辩过程管理">'6. 答辩组答辩过程管理'!$B$7</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="86">
   <si>
     <t>编号</t>
   </si>
@@ -480,12 +482,130 @@
   <si>
     <t>无</t>
   </si>
+  <si>
+    <t>教师用于管理自己已申报的课题，包括查看课题基础信息、查看学生的课题申请列表、下载学生提交的申请材料，并对学生申请进行“通过 / 拒绝”的处理。</t>
+  </si>
+  <si>
+    <t>1.教师只能管理自己申报的课题，不可查看他人课题
+2.每个课题可被多个学生申请
+3.学生申请一旦被教师“通过”，其他学生申请将自动失效
+4.教师对学生申请的“通过/拒绝”操作提交后不可撤销。
+5.学生必须提交申请材料文件，否则教师无法进行审核操作。</t>
+  </si>
+  <si>
+    <t>教师已经成功申报课题，并且教科办已开放学生选题申请入口。</t>
+  </si>
+  <si>
+    <t>1.页面初始化显示教师名下所有课题卡片（课题名称、类型、面向专业、剩余名额、申请中学生数量）。
+2.展示完整课题信息：课题类别（如：论文类）、面向专业、剩余名额、课题文件下载
+3.点击“学生课题申请”进入该课题的学生申请列表页面。
+4.在学生申请列表中可查看：学号、姓名、学生专业、学生提交的申请材料文件（可下载）
+5.教师可对每个学生进行操作：通过、拒绝
+6.点击某个学生可进入“学生课题申请详情”界面，内容包括：学号、姓名、专业、申请材料下载、通过 / 拒绝按钮</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.可折叠 / 展开课题卡片以节省空间。
+</t>
+  </si>
+  <si>
+    <t>1.〖学生申请审核〗“通过”成功，提示：“已通过该学生的选题申请”。
+2.〖学生申请审核〗“拒绝”成功，提示：“已拒绝该学生的选题申请”。
+3.〖申请审核〗失败（名额已满），提示：“该课题名额已满，无法再通过新的申请”。
+4.〖课题文件下载〗失败，提示：“课题文件不存在或已被删除”。
+5.〖学生申请文件下载〗失败，提示：“课题文件不存在或已被删除”。</t>
+  </si>
+  <si>
+    <t>1.教师不能操作不属于自己的课题。
+2.当课题剩余名额为 0 时，不允许对学生申请执行“通过”操作。
+3.已审核（通过/拒绝）的记录不可修改。
+4.学生申请材料需存在文件后才能进入审核步骤。</t>
+  </si>
+  <si>
+    <t>&lt;教师对学生申请的审核操作（通过 / 拒绝）&gt;</t>
+  </si>
+  <si>
+    <t>&lt;课题信息（课题名称、类型、面向专业、剩余名额）&gt; &lt;学生申请列表&gt; &lt;申请材料文件&gt; &lt;学生专业、姓名、学号&gt;&lt;审核结果显示&gt;</t>
+  </si>
+  <si>
+    <t>1.教师审核学生选题申请的完整性与及时性
+2.每个课题的申请数量、已通过数量、剩余名额变化</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>【</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>性能需求</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>】</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">：
+ 普通响应类  响应时间≤3秒
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>【</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>安全需求</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>】</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：
+ 1、操作权限：只有指导教师才能操作此功能项，并具有完整的操作权限
+ 2、数据权限：指导教师只能浏览或操作自己的申报表</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -577,6 +697,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -680,7 +810,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -711,83 +841,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1129,7 +1268,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1154,7 +1293,7 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="9"/>
@@ -1172,7 +1311,7 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="9"/>
@@ -1181,7 +1320,7 @@
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="9"/>
@@ -1199,7 +1338,7 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="9"/>
@@ -1283,6 +1422,7 @@
     <hyperlink ref="B2" location="表_学生选题" display="学生选题" xr:uid="{17DA5095-4D65-4699-8528-4656DF7030E9}"/>
     <hyperlink ref="B4" location="表_教师课题申报" display="教师课题申报" xr:uid="{7EC763B0-E7AD-4B8A-881F-543F4C803574}"/>
     <hyperlink ref="B7" location="表_答辩组答辩过程管理" display="答辩组答辩过程管理" xr:uid="{EA56FBFF-1865-460C-9D80-6681951686B3}"/>
+    <hyperlink ref="B5" location="表_教师选题管理" display="教师选题管理" xr:uid="{9B83E62A-97EE-4DA3-BB60-14FA991493DB}"/>
   </hyperlinks>
   <pageMargins left="0.69861111111111096" right="0.69861111111111096" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter alignWithMargins="0"/>
@@ -1299,103 +1439,103 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="4.75" style="18" customWidth="1"/>
-    <col min="3" max="3" width="40.58203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="18" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="18"/>
+    <col min="1" max="2" width="4.75" style="11" customWidth="1"/>
+    <col min="3" max="3" width="40.58203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="11" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="13">
         <v>45981</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="13">
         <v>45988</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:10" ht="115.5" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:10" ht="99" customHeight="1">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1405,8 +1545,8 @@
       <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:10" ht="43" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="24" t="s">
@@ -1416,8 +1556,8 @@
       <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:10" ht="150.5" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="24" t="s">
@@ -1425,11 +1565,11 @@
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
-      <c r="J10" s="26"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="85.5" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -1439,72 +1579,564 @@
       <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="61" customHeight="1">
-      <c r="A13" s="23"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:10" ht="90" customHeight="1">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890727C4-1477-433F-AD80-359ACAC52319}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="4.75" style="11" customWidth="1"/>
+    <col min="3" max="3" width="40.58203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="11" customWidth="1"/>
+    <col min="5" max="5" width="40.58203125" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" customHeight="1">
+      <c r="A1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13">
+        <v>45981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A3" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="13">
+        <v>45988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1">
+      <c r="A4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:10" ht="57" customHeight="1">
+      <c r="A5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1">
+      <c r="A6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" ht="98.5" customHeight="1">
+      <c r="A8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:10" ht="41" customHeight="1">
+      <c r="A9" s="20"/>
+      <c r="B9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:10" ht="146" customHeight="1">
+      <c r="A10" s="20"/>
+      <c r="B10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" ht="65" customHeight="1">
+      <c r="A11" s="20"/>
+      <c r="B11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1">
+      <c r="A12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" ht="61" customHeight="1">
+      <c r="A13" s="20"/>
+      <c r="B13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1">
+      <c r="A14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="78" customHeight="1">
+      <c r="A15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1">
+      <c r="A16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0665A72C-4FD6-4594-AA07-9A0C917AC882}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="4.75" customWidth="1"/>
+    <col min="3" max="3" width="40.58203125" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="40.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" customHeight="1">
+      <c r="A1" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1">
+      <c r="A2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="40">
+        <v>45981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1">
+      <c r="A3" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="40">
+        <v>45257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+    </row>
+    <row r="5" spans="1:10" ht="57" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" ht="105" customHeight="1">
+      <c r="A8" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+    </row>
+    <row r="9" spans="1:10" ht="66" customHeight="1">
+      <c r="A9" s="31"/>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+    </row>
+    <row r="10" spans="1:10" ht="146" customHeight="1">
+      <c r="A10" s="31"/>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="65" customHeight="1">
+      <c r="A11" s="31"/>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1">
+      <c r="A12" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+    </row>
+    <row r="13" spans="1:10" ht="61" customHeight="1">
+      <c r="A13" s="31"/>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="1:10" ht="78" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -1535,254 +2167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890727C4-1477-433F-AD80-359ACAC52319}">
-  <dimension ref="A1:J17"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="4.75" style="18" customWidth="1"/>
-    <col min="3" max="3" width="40.58203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="18" customWidth="1"/>
-    <col min="5" max="5" width="40.58203125" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="18"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1">
-      <c r="A1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="21">
-        <v>45981</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="21">
-        <v>45988</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1">
-      <c r="A4" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" spans="1:10" ht="57" customHeight="1">
-      <c r="A5" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1">
-      <c r="A6" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1">
-      <c r="A7" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:10" ht="98.5" customHeight="1">
-      <c r="A8" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:10" ht="41" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:10" ht="146" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="J10" s="26"/>
-    </row>
-    <row r="11" spans="1:10" ht="65" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:10" ht="61" customHeight="1">
-      <c r="A13" s="23"/>
-      <c r="B13" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1">
-      <c r="A14" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:10" ht="78" customHeight="1">
-      <c r="A15" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1">
-      <c r="A16" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8082CF-8FF2-4E0D-A89D-61E60BC40C3B}">
   <dimension ref="A1:J17"/>
   <sheetViews>
@@ -1792,50 +2177,50 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="4.75" style="38" customWidth="1"/>
-    <col min="3" max="3" width="40.58203125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="38" customWidth="1"/>
-    <col min="5" max="5" width="40.58203125" style="38" customWidth="1"/>
+    <col min="1" max="2" width="4.75" style="18" customWidth="1"/>
+    <col min="3" max="3" width="40.58203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="18" customWidth="1"/>
+    <col min="5" max="5" width="40.58203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="31"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="17">
         <v>45981</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="17">
         <v>45988</v>
       </c>
     </row>
@@ -1843,163 +2228,176 @@
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:10" ht="57" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="31"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="31"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="8" spans="1:10" ht="105" customHeight="1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="31"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
     </row>
     <row r="9" spans="1:10" ht="66" customHeight="1">
-      <c r="A9" s="36"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="31"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:10" ht="146" customHeight="1">
-      <c r="A10" s="36"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="65" customHeight="1">
-      <c r="A11" s="37"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="31"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="31" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="31"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
     </row>
     <row r="13" spans="1:10" ht="61" customHeight="1">
-      <c r="A13" s="37"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="31"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="31"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:10" ht="78" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="31"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="31"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="31"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="C12:E12"/>
@@ -2007,19 +2405,6 @@
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
docs(progress/week_10): remove placeholders for feature output
</commit_message>
<xml_diff>
--- a/docs/progress/week_10/功能分析表.xlsx
+++ b/docs/progress/week_10/功能分析表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29517"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29525"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\hdu2025_software_eng_thesis_mgmt\docs\progress\week_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD535F46-1422-4F0B-B22A-591CA18ADFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B06CF7-9F7C-4CBF-BB3D-B970A60FDAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="721" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="功能项清单" sheetId="9" r:id="rId1"/>
@@ -101,10 +101,6 @@
     <t>输出信息</t>
   </si>
   <si>
-    <t>&lt;功能项TITLE&gt;、&lt;课题面向专业&gt;、&lt;课题申报截止时间&gt;、&lt;题目名称&gt;、&lt;题目类型&gt;、&lt;毕业设计（论文）要求解决的问题及重点等&gt;、&lt;课题审核结果&gt;
-《毕业设计（论文）题目申报表》</t>
-  </si>
-  <si>
     <t>考核要素</t>
   </si>
   <si>
@@ -206,10 +202,6 @@
   </si>
   <si>
     <t>&lt;学生学号&gt;、&lt;学生姓名&gt;、&lt;所属专业&gt;、&lt;选题批次&gt;、&lt;课题编号&gt;、&lt;课题名称&gt;、&lt;课题类型&gt;、&lt;课题面向专业&gt;、&lt;指导教师姓名&gt;、&lt;毕业设计（论文）要求解决的问题及重点等&gt;、&lt;选题确认标志&gt; 等。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;功能项TITLE&gt;、&lt;学生基本信息（学号、姓名、专业等）&gt;、&lt;选题批次信息&gt;、&lt;课题名称&gt;、&lt;课题类型&gt;、&lt;课题面向专业&gt;、&lt;毕业设计（论文）要求解决的问题及重点等&gt;、&lt;指导教师姓名&gt;、&lt;当前选题状态&gt;、&lt;选题申请/确认时间&gt; </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -464,9 +456,6 @@
     <t>&lt;答辩分数&gt;、&lt;答辩意见&gt;</t>
   </si>
   <si>
-    <t>&lt;学生基本信息&gt;、&lt;提交文件名称&gt;、&lt;当前答辩状态&gt;、&lt;分数&gt;、&lt;答辩意见&gt;</t>
-  </si>
-  <si>
     <t>对学生答辩材料的审阅、评分与提交流程的规范性与完整性。</t>
   </si>
   <si>
@@ -522,9 +511,6 @@
   </si>
   <si>
     <t>&lt;教师对学生申请的审核操作（通过 / 拒绝）&gt;</t>
-  </si>
-  <si>
-    <t>&lt;课题信息（课题名称、类型、面向专业、剩余名额）&gt; &lt;学生申请列表&gt; &lt;申请材料文件&gt; &lt;学生专业、姓名、学号&gt;&lt;审核结果显示&gt;</t>
   </si>
   <si>
     <t>1.教师审核学生选题申请的完整性与及时性
@@ -599,6 +585,19 @@
  1、操作权限：只有指导教师才能操作此功能项，并具有完整的操作权限
  2、数据权限：指导教师只能浏览或操作自己的申报表</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;功能项：学生选题&gt;、&lt;学生基本信息（学号、姓名、专业等）&gt;、&lt;选题批次信息&gt;、&lt;课题名称&gt;、&lt;课题类型&gt;、&lt;课题面向专业&gt;、&lt;毕业设计（论文）要求解决的问题及重点等&gt;、&lt;指导教师姓名&gt;、&lt;当前选题状态&gt;、&lt;选题申请/确认时间&gt; </t>
+  </si>
+  <si>
+    <t>&lt;功能项：教师课题申报&gt;、&lt;课题面向专业&gt;、&lt;课题申报截止时间&gt;、&lt;题目名称&gt;、&lt;题目类型&gt;、&lt;毕业设计（论文）要求解决的问题及重点等&gt;、&lt;课题审核结果&gt;
+《毕业设计（论文）题目申报表》</t>
+  </si>
+  <si>
+    <t>&lt;功能项：答辩组答辩过程管理&gt;、&lt;学生基本信息&gt;、&lt;提交文件名称&gt;、&lt;当前答辩状态&gt;、&lt;分数&gt;、&lt;答辩意见&gt;</t>
+  </si>
+  <si>
+    <t>&lt;功能项：教师选题管理&gt; &lt;课题信息（课题名称、类型、面向专业、剩余名额）&gt; &lt;学生申请列表&gt; &lt;申请材料文件&gt; &lt;学生专业、姓名、学号&gt; &lt;审核结果显示&gt;</t>
   </si>
 </sst>
 </file>
@@ -810,7 +809,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -866,14 +865,26 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -881,51 +892,57 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1267,7 +1284,7 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1294,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="9"/>
     </row>
@@ -1303,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="9"/>
     </row>
@@ -1312,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="9"/>
     </row>
@@ -1321,7 +1338,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="9"/>
     </row>
@@ -1330,7 +1347,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -1339,7 +1356,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="9"/>
     </row>
@@ -1348,7 +1365,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="9"/>
     </row>
@@ -1433,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCA8D13-213D-4B02-BAF1-0986FDD6785D}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:E15"/>
+    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1447,23 +1464,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="19" t="s">
-        <v>31</v>
+      <c r="B1" s="22"/>
+      <c r="C1" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>5</v>
@@ -1473,12 +1490,12 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="28" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>7</v>
@@ -1491,8 +1508,8 @@
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>38</v>
+      <c r="B4" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -1502,8 +1519,8 @@
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>39</v>
+      <c r="B5" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
@@ -1513,8 +1530,8 @@
       <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>40</v>
+      <c r="B6" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -1524,90 +1541,90 @@
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="99" customHeight="1">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:10" ht="43" customHeight="1">
-      <c r="A9" s="20"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:10" ht="150.5" customHeight="1">
-      <c r="A10" s="20"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="85.5" customHeight="1">
-      <c r="A11" s="20"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>46</v>
+      <c r="C12" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="61" customHeight="1">
-      <c r="A13" s="20"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="C13" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -1615,36 +1632,528 @@
     </row>
     <row r="15" spans="1:10" ht="90" customHeight="1">
       <c r="A15" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1">
       <c r="A17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890727C4-1477-433F-AD80-359ACAC52319}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="4.75" style="11" customWidth="1"/>
+    <col min="3" max="3" width="40.58203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="11" customWidth="1"/>
+    <col min="5" max="5" width="40.58203125" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" customHeight="1">
+      <c r="A1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1">
+      <c r="A2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13">
+        <v>45981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="13">
+        <v>45988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1">
+      <c r="A4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:10" ht="57" customHeight="1">
+      <c r="A5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1">
+      <c r="A6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" ht="98.5" customHeight="1">
+      <c r="A8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:10" ht="41" customHeight="1">
+      <c r="A9" s="23"/>
+      <c r="B9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:10" ht="146" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" ht="65" customHeight="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1">
+      <c r="A12" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" ht="61" customHeight="1">
+      <c r="A13" s="23"/>
+      <c r="B13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1">
+      <c r="A14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="78" customHeight="1">
+      <c r="A15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1">
+      <c r="A16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0665A72C-4FD6-4594-AA07-9A0C917AC882}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="4.75" customWidth="1"/>
+    <col min="3" max="3" width="40.58203125" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="40.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" customHeight="1">
+      <c r="A1" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1">
+      <c r="A2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="19">
+        <v>45981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1">
+      <c r="A3" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="19">
+        <v>45257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" ht="57" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:10" ht="105" customHeight="1">
+      <c r="A8" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+    </row>
+    <row r="9" spans="1:10" ht="66" customHeight="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="1:10" ht="146" customHeight="1">
+      <c r="A10" s="30"/>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="65" customHeight="1">
+      <c r="A11" s="30"/>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1">
+      <c r="A12" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+    </row>
+    <row r="13" spans="1:10" ht="61" customHeight="1">
+      <c r="A13" s="30"/>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+    </row>
+    <row r="15" spans="1:10" ht="78" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -1675,468 +2184,221 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890727C4-1477-433F-AD80-359ACAC52319}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8082CF-8FF2-4E0D-A89D-61E60BC40C3B}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="4.75" style="11" customWidth="1"/>
-    <col min="3" max="3" width="40.58203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="11" customWidth="1"/>
-    <col min="5" max="5" width="40.58203125" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="11"/>
+    <col min="1" max="2" width="4.75" style="18" customWidth="1"/>
+    <col min="3" max="3" width="40.58203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="18" customWidth="1"/>
+    <col min="5" max="5" width="40.58203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="13">
-        <v>45981</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A3" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="13">
-        <v>45988</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1">
-      <c r="A4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:10" ht="57" customHeight="1">
-      <c r="A5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1">
-      <c r="A6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1">
-      <c r="A7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-    </row>
-    <row r="8" spans="1:10" ht="98.5" customHeight="1">
-      <c r="A8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:10" ht="41" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:10" ht="146" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:10" ht="65" customHeight="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13" spans="1:10" ht="61" customHeight="1">
-      <c r="A13" s="20"/>
-      <c r="B13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1">
-      <c r="A14" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="1:10" ht="78" customHeight="1">
-      <c r="A15" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1">
-      <c r="A16" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0665A72C-4FD6-4594-AA07-9A0C917AC882}">
-  <dimension ref="A1:J17"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="4.75" customWidth="1"/>
-    <col min="3" max="3" width="40.58203125" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="40.58203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1">
-      <c r="A1" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="17">
         <v>45981</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="35" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="40">
-        <v>45257</v>
+      <c r="E3" s="17">
+        <v>45988</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>75</v>
+      <c r="B4" s="29" t="s">
+        <v>59</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="57" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
+      <c r="B5" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>12</v>
+      <c r="B6" s="29" t="s">
+        <v>61</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
+      <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:10" ht="105" customHeight="1">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
+      <c r="C8" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="66" customHeight="1">
-      <c r="A9" s="31"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
+      <c r="C9" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" spans="1:10" ht="146" customHeight="1">
-      <c r="A10" s="31"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="C10" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="65" customHeight="1">
-      <c r="A11" s="31"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="C11" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>82</v>
+      <c r="C12" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="13" spans="1:10" ht="61" customHeight="1">
-      <c r="A13" s="31"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
+      <c r="C13" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="46"/>
+      <c r="E13" s="47"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>84</v>
+        <v>23</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+      <c r="E14" s="38"/>
     </row>
     <row r="15" spans="1:10" ht="78" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>85</v>
+        <v>25</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>69</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+      <c r="E15" s="38"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
+        <v>26</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="38"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+        <v>28</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -2154,257 +2416,12 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:E11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8082CF-8FF2-4E0D-A89D-61E60BC40C3B}">
-  <dimension ref="A1:J17"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="4.75" style="18" customWidth="1"/>
-    <col min="3" max="3" width="40.58203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="18" customWidth="1"/>
-    <col min="5" max="5" width="40.58203125" style="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1">
-      <c r="A1" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="17">
-        <v>45981</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18" customHeight="1">
-      <c r="A3" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="17">
-        <v>45988</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
-    </row>
-    <row r="5" spans="1:10" ht="57" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="37"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:10" ht="105" customHeight="1">
-      <c r="A8" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" spans="1:10" ht="66" customHeight="1">
-      <c r="A9" s="34"/>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" spans="1:10" ht="146" customHeight="1">
-      <c r="A10" s="34"/>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" ht="65" customHeight="1">
-      <c r="A11" s="32"/>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
-    </row>
-    <row r="13" spans="1:10" ht="61" customHeight="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-    </row>
-    <row r="15" spans="1:10" ht="78" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
docs(progress/week_10): add more features
Closes: #17
Signed-off-by: Rong "Mantle" Bao <webmaster@csmantle.top>
</commit_message>
<xml_diff>
--- a/docs/progress/week_10/功能分析表.xlsx
+++ b/docs/progress/week_10/功能分析表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\hdu2025_software_eng_thesis_mgmt\docs\progress\week_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B06CF7-9F7C-4CBF-BB3D-B970A60FDAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAF5095-D465-40D0-A2B8-E4943BD11BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="721" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="功能项清单" sheetId="9" r:id="rId1"/>
@@ -18,19 +18,21 @@
     <sheet name="3. 教师课题申报" sheetId="23" r:id="rId3"/>
     <sheet name="4. 教师选题管理" sheetId="25" r:id="rId4"/>
     <sheet name="6. 答辩组答辩过程管理" sheetId="24" r:id="rId5"/>
+    <sheet name="7. 教课办课题管理" sheetId="26" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="表_学生选题">'1. 学生选题'!$A$1</definedName>
     <definedName name="表_教师课题申报">'3. 教师课题申报'!$A$1</definedName>
-    <definedName name="表_教师选题管理">'4. 教师选题管理'!$C$1</definedName>
-    <definedName name="表_答辩组答辩过程管理">'6. 答辩组答辩过程管理'!$B$7</definedName>
+    <definedName name="表_教师选题管理">'4. 教师选题管理'!$A$1</definedName>
+    <definedName name="表_教科办课题管理">'7. 教课办课题管理'!$A$1</definedName>
+    <definedName name="表_答辩组答辩过程管理">'6. 答辩组答辩过程管理'!$A$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="102">
   <si>
     <t>编号</t>
   </si>
@@ -599,12 +601,87 @@
   <si>
     <t>&lt;功能项：教师选题管理&gt; &lt;课题信息（课题名称、类型、面向专业、剩余名额）&gt; &lt;学生申请列表&gt; &lt;申请材料文件&gt; &lt;学生专业、姓名、学号&gt; &lt;审核结果显示&gt;</t>
   </si>
+  <si>
+    <t>教课办课题管理</t>
+  </si>
+  <si>
+    <t>罗传杰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗传杰</t>
+  </si>
+  <si>
+    <t>教科办负责申报流程的启动、课题的发布、对教师申报课题进行审核（含原审核组职责）、管理学生申报资格、汇总最终申报结果并发布。</t>
+  </si>
+  <si>
+    <t>1. 课题申报必须在教科办申报通知中规定的时间内完成申请与确认，超出时间不予受理。
+2. 每个老师可以申报多个课题
+3. 课题申报一经确认（通过教科办审核并确认），教师不得在系统中自行更换或退选，如需变更需线下办理并由教科办处理。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教科办</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教科办先发布课题申报通知，教师开始课题申报。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.页面初始化，显示所有课题的列表，并默认显示课题的基本信息（&lt;课题名称&gt;、&lt;课题类型&gt;、&lt;指导教师&gt;、&lt;审核状态&gt;）。
+2. 批量或单个查看、审核教师申报的课题，并填写&lt;审核意见&gt;。审核结果包括“通过”、“不通过”。
+3. 汇总教师对学生申报的处理结果（允许/拒绝），生成&lt;最终申报结果名单&gt;。
+4. 公布&lt;通过审核的课题清单&gt;。</t>
+  </si>
+  <si>
+    <t>1. 能够按课题名称、关键字或指导教师姓名对课题进行模糊搜索及快速定位。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 〖申报申请〗操作成功完成，提示“已成功提交对课题：…… 的申报申请”
+2. 〖申报修改〗（审批状态修改）操作成功完成，提示“已成功修改申报审批状态：……”
+3. 〖申报内容修改〗操作成功完成，提示“已成功修改对课题…… 的申报申请”
+4. 〖申报确认〗操作成功完成，提示“毕业设计申报已确认，确认时间：……””
+5. 〖申报申请〗操作失败（超出截止时间），提示“申报已过截止时间，无法提交/确认！”
+6. 〖申报修改〗操作失败（超出截止时间）操作成功完成，提示“申报已过截止时间，无法提交/确认！”
+7. 〖申报内容修改〗操作失败（超出截止时间），提示“申报已过截止时间，无法提交/确认！”
+8. 〖申报确认〗操作失败（超出截止时间），提示“申报已过截止时间，无法提交/确认！”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 检测系统时间与申报截止时间，当达到或超出截止时间时，不允许提交新的申报申请、确认或修改，并提示用户
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;所属专业&gt;、&lt;申报批次&gt;、&lt;课题编号&gt;、&lt;课题名称&gt;、&lt;课题类型&gt;、&lt;课题面向专业&gt;、&lt;指导教师姓名&gt;、&lt;毕业设计（论文）要求解决的问题及重点等&gt;、&lt;申报确认标志&gt; 等。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;功能项TITLE&gt;、&lt;申报批次信息&gt;、&lt;课题名称&gt;、&lt;课题类型&gt;、&lt;课题面向专业&gt;、&lt;毕业设计（论文）要求解决的问题及重点等&gt;、&lt;指导教师姓名&gt;、&lt;当前申报状态&gt;、&lt;申报申请/确认时间&gt; </t>
+  </si>
+  <si>
+    <t>是否严格按照时间窗口与数量约束完成申报。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>【性能需求】：
+普通响应类 响应时间 ≤ 3 秒
+【安全需求】：
+1.操作权限：只有教科办能够修改审批状态。
+2.数据权限：只有教科办能够访问相关申报课题的相关数据。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申报课题数量统计（包括课题通过数、分专业课题通过数等）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -707,6 +784,11 @@
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -809,7 +891,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -943,6 +1025,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1284,8 +1372,8 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1364,7 +1452,7 @@
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="9"/>
@@ -1440,6 +1528,7 @@
     <hyperlink ref="B4" location="表_教师课题申报" display="教师课题申报" xr:uid="{7EC763B0-E7AD-4B8A-881F-543F4C803574}"/>
     <hyperlink ref="B7" location="表_答辩组答辩过程管理" display="答辩组答辩过程管理" xr:uid="{EA56FBFF-1865-460C-9D80-6681951686B3}"/>
     <hyperlink ref="B5" location="表_教师选题管理" display="教师选题管理" xr:uid="{9B83E62A-97EE-4DA3-BB60-14FA991493DB}"/>
+    <hyperlink ref="B8" location="表_教科办课题管理" display="教科办课题管理" xr:uid="{1CC904B5-6C1B-4080-A1AE-C215CD7946EC}"/>
   </hyperlinks>
   <pageMargins left="0.69861111111111096" right="0.69861111111111096" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter alignWithMargins="0"/>
@@ -1943,7 +2032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0665A72C-4FD6-4594-AA07-9A0C917AC882}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:E14"/>
     </sheetView>
   </sheetViews>
@@ -2188,7 +2277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8082CF-8FF2-4E0D-A89D-61E60BC40C3B}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C13" sqref="C13:E13"/>
     </sheetView>
   </sheetViews>
@@ -2426,4 +2515,250 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8342AB7-A215-4703-9B77-A503A5539868}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="4.75" style="11" customWidth="1"/>
+    <col min="3" max="3" width="40.58203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="11" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" customHeight="1">
+      <c r="A1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1">
+      <c r="A2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13">
+        <v>45988</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28" customHeight="1">
+      <c r="A3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="13">
+        <v>45988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1">
+      <c r="A4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:10" ht="115.5" customHeight="1">
+      <c r="A5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1">
+      <c r="A6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" ht="99" customHeight="1">
+      <c r="A8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" ht="43" customHeight="1">
+      <c r="A9" s="23"/>
+      <c r="B9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" ht="150.65" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="J10" s="48"/>
+    </row>
+    <row r="11" spans="1:10" ht="85.5" customHeight="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1">
+      <c r="A12" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" ht="61" customHeight="1">
+      <c r="A13" s="23"/>
+      <c r="B13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1">
+      <c r="A14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="90" customHeight="1">
+      <c r="A15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1">
+      <c r="A16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111096" footer="0.51111111111111096"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>